<commit_message>
Update add asset for master currency & transaction type
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\Sprint 3 Bucket\Traveloka_DataAutomation_Performer_Bucket\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC7076A-5563-4A61-BDED-612E4F563E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF28D2C8-3073-4B35-85AA-AEADC77841BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23232" windowHeight="11496" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14790" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
   <si>
     <t>Name</t>
   </si>
@@ -183,9 +183,6 @@
     <t>[Dev] RPA_Moon_PathMailTemplate</t>
   </si>
   <si>
-    <t>ConverterPath</t>
-  </si>
-  <si>
     <t>RPA_Moon_AutoRetryMax</t>
   </si>
   <si>
@@ -198,9 +195,6 @@
     <t>AutoRetryPostpone</t>
   </si>
   <si>
-    <t>[Dev] RPA_Moon_PathExcel</t>
-  </si>
-  <si>
     <t>[Dev] RPA_Moon_Cred_Gmail</t>
   </si>
   <si>
@@ -226,6 +220,30 @@
   </si>
   <si>
     <t>[Dev] RPA_Moon_Bucket</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_SheetIdConfig_Treasury</t>
+  </si>
+  <si>
+    <t>SheetIdConfig_Treasury</t>
+  </si>
+  <si>
+    <t>RPA209_VCC_Citibank_MasterCurrencyCode</t>
+  </si>
+  <si>
+    <t>RPA209_VCC_Citibank_MasterTransactionType</t>
+  </si>
+  <si>
+    <t>MasterCurrencyCode</t>
+  </si>
+  <si>
+    <t>MasterTransactionType</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_PathSaKey</t>
+  </si>
+  <si>
+    <t>PathSaKey</t>
   </si>
 </sst>
 </file>
@@ -305,9 +323,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -345,7 +363,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -451,7 +469,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -593,7 +611,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -654,7 +672,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -686,7 +704,7 @@
         <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.3" customHeight="1">
@@ -702,15 +720,15 @@
         <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.3" customHeight="1">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.3" customHeight="1">
@@ -2880,10 +2898,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="14.95" customHeight="1"/>
@@ -2948,55 +2966,69 @@
     </row>
     <row r="4" spans="1:26" ht="14.3" customHeight="1">
       <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
         <v>52</v>
-      </c>
-      <c r="B4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.3" customHeight="1">
       <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
         <v>54</v>
-      </c>
-      <c r="B5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.3" customHeight="1">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.3" customHeight="1">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.3" customHeight="1">
-      <c r="A8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" t="s">
-        <v>60</v>
+      <c r="A8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.3" customHeight="1">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="14.3" customHeight="1">
-      <c r="A10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:26" ht="14.3" customHeight="1">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="D11" s="4"/>
+      <c r="A11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:26" ht="14.3" customHeight="1">
       <c r="D12" s="2"/>
@@ -3037,9 +3069,7 @@
     <row r="24" spans="4:4" ht="14.3" customHeight="1">
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="4:4" ht="14.3" customHeight="1">
-      <c r="D25" s="2"/>
-    </row>
+    <row r="25" spans="4:4" ht="14.3" customHeight="1"/>
     <row r="26" spans="4:4" ht="14.3" customHeight="1"/>
     <row r="27" spans="4:4" ht="14.3" customHeight="1"/>
     <row r="28" spans="4:4" ht="14.3" customHeight="1"/>
@@ -4011,7 +4041,6 @@
     <row r="994" ht="14.3" customHeight="1"/>
     <row r="995" ht="14.3" customHeight="1"/>
     <row r="996" ht="14.3" customHeight="1"/>
-    <row r="997" ht="14.3" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>